<commit_message>
HEALTHKING php 명세서 추가, table 명세서 변경
</commit_message>
<xml_diff>
--- a/Teacher/Server/HEALTHKING Table 명세서.xlsx
+++ b/Teacher/Server/HEALTHKING Table 명세서.xlsx
@@ -439,12 +439,92 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -456,7 +536,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -465,6 +545,33 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -763,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -802,736 +909,798 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="C3" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="C4" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="E4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="E5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="C6" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="E6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="C7" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="E7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="E8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="C9" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="E9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="C10" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="E10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="C11" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="E11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="C12" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="E12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="C13" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="E13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="C14" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="E14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="C15" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="E15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="E16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="C17" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="E17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="C18" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="E18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="C19" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="E19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="C20" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="E20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="C21" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="E21" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="E22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="C23" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E23" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="E23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="C24" t="s">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E24" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="E24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="C25" t="s">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="E25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="C26" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E26" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="E26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="E27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="C28" t="s">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E28" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="E28" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="C29" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E29" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="E29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="C30" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E30" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="E30" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="E31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="C32" t="s">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E32" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="E32" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="C33" t="s">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E33" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="E33" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="C34" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="E34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="11" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" t="s">
+      <c r="A35" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E35" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="E35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="C36" t="s">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E36" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="E36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="C37" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E37" t="s">
-        <v>5</v>
-      </c>
-      <c r="F37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="E37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="C38" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E38" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="E38" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="11" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" t="s">
+      <c r="A39" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F39" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="E39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="C40" t="s">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E40" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="E40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="C41" t="s">
+      <c r="A41" s="9"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E41" t="s">
-        <v>5</v>
-      </c>
-      <c r="F41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="E41" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="11" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>